<commit_message>
Build project and update necessary files
</commit_message>
<xml_diff>
--- a/dist/产品库存及周转统计.xlsx
+++ b/dist/产品库存及周转统计.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28000" windowHeight="15800"/>
+    <workbookView windowHeight="20900"/>
   </bookViews>
   <sheets>
     <sheet name="产品库存" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">产品库存!$A$1:$AH$44</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">产品库存!$A$1:$AH$51</definedName>
   </definedNames>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
@@ -522,7 +522,7 @@
     <t>床边双大袋（灰）1p</t>
   </si>
   <si>
-    <t>B0DQGTP8MQ</t>
+    <t>BOFHHY887F</t>
   </si>
   <si>
     <t>14</t>
@@ -531,10 +531,10 @@
     <t>5</t>
   </si>
   <si>
-    <t>BedSideCaddy-2pockets-Grey1pcs</t>
-  </si>
-  <si>
-    <t>X004DUD277</t>
+    <t>BedSideCaddy-2pockets-Greyipcs-New</t>
+  </si>
+  <si>
+    <t>X004RETHGT</t>
   </si>
   <si>
     <t>【大】深卡其(2p)</t>
@@ -1460,7 +1460,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1532,9 +1532,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1937,11 +1934,11 @@
   <dimension ref="A1:AH71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="S33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="T7" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AA51" sqref="AA51"/>
+      <selection pane="bottomRight" activeCell="AE13" sqref="AE13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -1987,16 +1984,16 @@
       <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="24" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="I1" s="32" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="8" t="s">
@@ -2012,34 +2009,34 @@
       <c r="N1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="34" t="s">
+      <c r="O1" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="35" t="s">
+      <c r="Q1" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="35" t="s">
+      <c r="R1" s="34" t="s">
         <v>15</v>
       </c>
       <c r="T1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="36" t="s">
+      <c r="U1" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="36" t="s">
+      <c r="V1" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="36" t="s">
+      <c r="W1" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="36" t="s">
+      <c r="X1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="Y1" s="36" t="s">
+      <c r="Y1" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="36" t="s">
+      <c r="Z1" s="35" t="s">
         <v>22</v>
       </c>
       <c r="AD1" s="7" t="s">
@@ -2071,28 +2068,28 @@
       <c r="D2" s="9">
         <v>0</v>
       </c>
-      <c r="E2" s="27">
+      <c r="E2" s="26">
         <f t="shared" ref="E2:E51" si="0">C2+D2</f>
         <v>0</v>
       </c>
-      <c r="F2" s="28">
+      <c r="F2" s="27">
         <v>16.4</v>
       </c>
-      <c r="G2" s="29">
+      <c r="G2" s="28">
         <v>13.8</v>
       </c>
-      <c r="H2" s="26">
+      <c r="H2" s="25">
         <v>20.5</v>
       </c>
-      <c r="I2" s="26">
+      <c r="I2" s="25">
         <f t="shared" ref="I2:I19" si="1">MAX(F2,G2)*1.375</f>
         <v>22.55</v>
       </c>
-      <c r="J2" s="26">
+      <c r="J2" s="25">
         <f t="shared" ref="J2:J51" si="2">(C2)/I2</f>
         <v>0</v>
       </c>
-      <c r="K2" s="26">
+      <c r="K2" s="25">
         <f t="shared" ref="K2:K51" si="3">(E2)/I2</f>
         <v>0</v>
       </c>
@@ -2103,30 +2100,30 @@
       <c r="N2" s="17">
         <v>6</v>
       </c>
-      <c r="O2" s="34">
+      <c r="O2" s="33">
         <f t="shared" ref="O2:O45" si="4">M2+N2</f>
         <v>25.43</v>
       </c>
-      <c r="Q2" s="35">
+      <c r="Q2" s="34">
         <f t="shared" ref="Q2:Q45" si="5">M2*C2</f>
         <v>0</v>
       </c>
-      <c r="R2" s="35">
+      <c r="R2" s="34">
         <f t="shared" ref="R2:R45" si="6">M2*D2</f>
         <v>0</v>
       </c>
       <c r="T2" s="7">
         <v>36</v>
       </c>
-      <c r="U2" s="37"/>
-      <c r="V2" s="37"/>
-      <c r="W2" s="38">
+      <c r="U2" s="36"/>
+      <c r="V2" s="36"/>
+      <c r="W2" s="37">
         <f>CEILING(MAX(0,135-MAX(K2,60))*I2/T2,1)*T2</f>
         <v>1692</v>
       </c>
-      <c r="X2" s="37"/>
-      <c r="Y2" s="37"/>
-      <c r="Z2" s="38">
+      <c r="X2" s="36"/>
+      <c r="Y2" s="36"/>
+      <c r="Z2" s="37">
         <f>MIN(CEILING(MAX(0,115-MAX(J2,30))*I2/T2,1)*T2,D2)</f>
         <v>0</v>
       </c>
@@ -2159,28 +2156,28 @@
       <c r="D3" s="9">
         <v>0</v>
       </c>
-      <c r="E3" s="27">
+      <c r="E3" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F3" s="28">
+      <c r="F3" s="27">
         <v>5.7</v>
       </c>
-      <c r="G3" s="29">
+      <c r="G3" s="28">
         <v>5.3</v>
       </c>
-      <c r="H3" s="26">
+      <c r="H3" s="25">
         <v>8</v>
       </c>
-      <c r="I3" s="26">
+      <c r="I3" s="25">
         <f t="shared" si="1"/>
         <v>7.8375</v>
       </c>
-      <c r="J3" s="26">
+      <c r="J3" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K3" s="26">
+      <c r="K3" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2191,30 +2188,30 @@
       <c r="N3" s="17">
         <v>10</v>
       </c>
-      <c r="O3" s="34">
+      <c r="O3" s="33">
         <f t="shared" si="4"/>
         <v>34.37</v>
       </c>
-      <c r="Q3" s="35">
+      <c r="Q3" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R3" s="35">
+      <c r="R3" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T3" s="7">
         <v>32</v>
       </c>
-      <c r="U3" s="37"/>
-      <c r="V3" s="37"/>
-      <c r="W3" s="38">
+      <c r="U3" s="36"/>
+      <c r="V3" s="36"/>
+      <c r="W3" s="37">
         <f>CEILING(MAX(0,135-MAX(K3,60))*I3/T3,1)*T3</f>
         <v>608</v>
       </c>
-      <c r="X3" s="37"/>
-      <c r="Y3" s="37"/>
-      <c r="Z3" s="38">
+      <c r="X3" s="36"/>
+      <c r="Y3" s="36"/>
+      <c r="Z3" s="37">
         <f>MIN(CEILING(MAX(0,115-MAX(J3,30))*I3/T3,1)*T3,D3)</f>
         <v>0</v>
       </c>
@@ -2247,28 +2244,28 @@
       <c r="D4" s="9">
         <v>0</v>
       </c>
-      <c r="E4" s="27">
+      <c r="E4" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F4" s="28">
+      <c r="F4" s="27">
         <v>5.4</v>
       </c>
-      <c r="G4" s="29">
+      <c r="G4" s="28">
         <v>6.1</v>
       </c>
-      <c r="H4" s="26">
+      <c r="H4" s="25">
         <v>8</v>
       </c>
-      <c r="I4" s="26">
+      <c r="I4" s="25">
         <f t="shared" si="1"/>
         <v>8.3875</v>
       </c>
-      <c r="J4" s="26">
+      <c r="J4" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K4" s="26">
+      <c r="K4" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2279,30 +2276,30 @@
       <c r="N4" s="17">
         <v>6.98</v>
       </c>
-      <c r="O4" s="34">
+      <c r="O4" s="33">
         <f t="shared" si="4"/>
         <v>29.72</v>
       </c>
-      <c r="Q4" s="35">
+      <c r="Q4" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R4" s="35">
+      <c r="R4" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T4" s="7">
         <v>42</v>
       </c>
-      <c r="U4" s="37"/>
-      <c r="V4" s="37"/>
-      <c r="W4" s="38">
+      <c r="U4" s="36"/>
+      <c r="V4" s="36"/>
+      <c r="W4" s="37">
         <f>CEILING(MAX(0,135-MAX(K4,60))*I4/T4,1)*T4</f>
         <v>630</v>
       </c>
-      <c r="X4" s="37"/>
-      <c r="Y4" s="37"/>
-      <c r="Z4" s="38">
+      <c r="X4" s="36"/>
+      <c r="Y4" s="36"/>
+      <c r="Z4" s="37">
         <f>MIN(CEILING(MAX(0,115-MAX(J4,30))*I4/T4,1)*T4,D4)</f>
         <v>0</v>
       </c>
@@ -2335,28 +2332,28 @@
       <c r="D5" s="9">
         <v>0</v>
       </c>
-      <c r="E5" s="27">
+      <c r="E5" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F5" s="28">
+      <c r="F5" s="27">
         <v>10</v>
       </c>
-      <c r="G5" s="29">
+      <c r="G5" s="28">
         <v>11.5</v>
       </c>
-      <c r="H5" s="26">
+      <c r="H5" s="25">
         <v>17</v>
       </c>
-      <c r="I5" s="26">
+      <c r="I5" s="25">
         <f t="shared" si="1"/>
         <v>15.8125</v>
       </c>
-      <c r="J5" s="26">
+      <c r="J5" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K5" s="26">
+      <c r="K5" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2367,30 +2364,30 @@
       <c r="N5" s="17">
         <v>10</v>
       </c>
-      <c r="O5" s="34">
+      <c r="O5" s="33">
         <f t="shared" si="4"/>
         <v>34.37</v>
       </c>
-      <c r="Q5" s="35">
+      <c r="Q5" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R5" s="35">
+      <c r="R5" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T5" s="7">
         <v>32</v>
       </c>
-      <c r="U5" s="37"/>
-      <c r="V5" s="37"/>
-      <c r="W5" s="38">
+      <c r="U5" s="36"/>
+      <c r="V5" s="36"/>
+      <c r="W5" s="37">
         <f>CEILING(MAX(0,135-MAX(K5,60))*I5/T5,1)*T5</f>
         <v>1216</v>
       </c>
-      <c r="X5" s="37"/>
-      <c r="Y5" s="37"/>
-      <c r="Z5" s="38">
+      <c r="X5" s="36"/>
+      <c r="Y5" s="36"/>
+      <c r="Z5" s="37">
         <f>MIN(CEILING(MAX(0,115-MAX(J5,30))*I5/T5,1)*T5,D5)</f>
         <v>0</v>
       </c>
@@ -2423,28 +2420,28 @@
       <c r="D6" s="9">
         <v>0</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F6" s="28">
+      <c r="F6" s="27">
         <v>9.2</v>
       </c>
-      <c r="G6" s="29">
+      <c r="G6" s="28">
         <v>9.4</v>
       </c>
-      <c r="H6" s="26">
+      <c r="H6" s="25">
         <v>13.5</v>
       </c>
-      <c r="I6" s="26">
+      <c r="I6" s="25">
         <f t="shared" si="1"/>
         <v>12.925</v>
       </c>
-      <c r="J6" s="26">
+      <c r="J6" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K6" s="26">
+      <c r="K6" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2455,30 +2452,30 @@
       <c r="N6" s="17">
         <v>10</v>
       </c>
-      <c r="O6" s="34">
+      <c r="O6" s="33">
         <f t="shared" si="4"/>
         <v>36.57</v>
       </c>
-      <c r="Q6" s="35">
+      <c r="Q6" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R6" s="35">
+      <c r="R6" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T6" s="7">
         <v>32</v>
       </c>
-      <c r="U6" s="37"/>
-      <c r="V6" s="37"/>
-      <c r="W6" s="38">
+      <c r="U6" s="36"/>
+      <c r="V6" s="36"/>
+      <c r="W6" s="37">
         <f>CEILING(MAX(0,135-MAX(K6,60))*I6/T6,1)*T6</f>
         <v>992</v>
       </c>
-      <c r="X6" s="37"/>
-      <c r="Y6" s="37"/>
-      <c r="Z6" s="38">
+      <c r="X6" s="36"/>
+      <c r="Y6" s="36"/>
+      <c r="Z6" s="37">
         <f>MIN(CEILING(MAX(0,115-MAX(J6,30))*I6/T6,1)*T6,D6)</f>
         <v>0</v>
       </c>
@@ -2511,28 +2508,28 @@
       <c r="D7" s="9">
         <v>0</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="27">
         <v>1</v>
       </c>
-      <c r="G7" s="29">
+      <c r="G7" s="28">
         <v>1.3</v>
       </c>
-      <c r="H7" s="26">
+      <c r="H7" s="25">
         <v>2.5</v>
       </c>
-      <c r="I7" s="26">
+      <c r="I7" s="25">
         <f t="shared" si="1"/>
         <v>1.7875</v>
       </c>
-      <c r="J7" s="26">
+      <c r="J7" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K7" s="26">
+      <c r="K7" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2543,33 +2540,33 @@
       <c r="N7" s="17">
         <v>13.38</v>
       </c>
-      <c r="O7" s="34">
+      <c r="O7" s="33">
         <f t="shared" si="4"/>
         <v>49.49</v>
       </c>
-      <c r="Q7" s="35">
+      <c r="Q7" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R7" s="35">
+      <c r="R7" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T7" s="7">
         <v>12</v>
       </c>
-      <c r="U7" s="37"/>
-      <c r="V7" s="38">
+      <c r="U7" s="36"/>
+      <c r="V7" s="37">
         <f>CEILING(MAX(0,120-MAX(K7,60))*I7/T7,1)*T7</f>
         <v>108</v>
       </c>
-      <c r="W7" s="37"/>
-      <c r="X7" s="37"/>
-      <c r="Y7" s="38">
+      <c r="W7" s="36"/>
+      <c r="X7" s="36"/>
+      <c r="Y7" s="37">
         <f>MIN(CEILING(MAX(0,100-MAX(J7,30))*I7/T7,1)*T7,D7)</f>
         <v>0</v>
       </c>
-      <c r="Z7" s="37"/>
+      <c r="Z7" s="36"/>
       <c r="AD7" s="7" t="s">
         <v>50</v>
       </c>
@@ -2599,29 +2596,29 @@
       <c r="D8" s="9">
         <v>0</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F8" s="28">
+      <c r="F8" s="27">
         <v>1.7</v>
       </c>
-      <c r="G8" s="29">
+      <c r="G8" s="28">
         <v>1.6</v>
       </c>
-      <c r="H8" s="26">
+      <c r="H8" s="25">
         <f t="shared" ref="H8:H14" si="7">MAX(E8,F8)*1.375</f>
         <v>2.3375</v>
       </c>
-      <c r="I8" s="26">
+      <c r="I8" s="25">
         <f t="shared" si="1"/>
         <v>2.3375</v>
       </c>
-      <c r="J8" s="26">
+      <c r="J8" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K8" s="26">
+      <c r="K8" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2632,33 +2629,33 @@
       <c r="N8" s="17">
         <v>10.47</v>
       </c>
-      <c r="O8" s="34">
+      <c r="O8" s="33">
         <f t="shared" si="4"/>
         <v>44.18</v>
       </c>
-      <c r="Q8" s="35">
+      <c r="Q8" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R8" s="35">
+      <c r="R8" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T8" s="7">
         <v>15</v>
       </c>
-      <c r="U8" s="37"/>
-      <c r="V8" s="38">
+      <c r="U8" s="36"/>
+      <c r="V8" s="37">
         <f t="shared" ref="V8:V15" si="8">CEILING(MAX(0,120-MAX(K8,60))*I8/T8,1)*T8</f>
         <v>150</v>
       </c>
-      <c r="W8" s="37"/>
-      <c r="X8" s="37"/>
-      <c r="Y8" s="38">
+      <c r="W8" s="36"/>
+      <c r="X8" s="36"/>
+      <c r="Y8" s="37">
         <f t="shared" ref="Y8:Y15" si="9">MIN(CEILING(MAX(0,100-MAX(J8,30))*I8/T8,1)*T8,D8)</f>
         <v>0</v>
       </c>
-      <c r="Z8" s="37"/>
+      <c r="Z8" s="36"/>
       <c r="AD8" s="7" t="s">
         <v>54</v>
       </c>
@@ -2688,28 +2685,28 @@
       <c r="D9" s="9">
         <v>0</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F9" s="28">
+      <c r="F9" s="27">
         <v>1.7</v>
       </c>
-      <c r="G9" s="29">
+      <c r="G9" s="28">
         <v>1.3</v>
       </c>
-      <c r="H9" s="26">
+      <c r="H9" s="25">
         <v>5</v>
       </c>
-      <c r="I9" s="26">
+      <c r="I9" s="25">
         <f t="shared" si="1"/>
         <v>2.3375</v>
       </c>
-      <c r="J9" s="26">
+      <c r="J9" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K9" s="26">
+      <c r="K9" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2720,33 +2717,33 @@
       <c r="N9" s="17">
         <v>9</v>
       </c>
-      <c r="O9" s="34">
+      <c r="O9" s="33">
         <f t="shared" si="4"/>
         <v>37.52</v>
       </c>
-      <c r="Q9" s="35">
+      <c r="Q9" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R9" s="35">
+      <c r="R9" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T9" s="7">
         <v>28</v>
       </c>
-      <c r="U9" s="37"/>
-      <c r="V9" s="38">
+      <c r="U9" s="36"/>
+      <c r="V9" s="37">
         <f t="shared" si="8"/>
         <v>168</v>
       </c>
-      <c r="W9" s="37"/>
-      <c r="X9" s="37"/>
-      <c r="Y9" s="38">
+      <c r="W9" s="36"/>
+      <c r="X9" s="36"/>
+      <c r="Y9" s="37">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="Z9" s="37"/>
+      <c r="Z9" s="36"/>
       <c r="AD9" s="7" t="s">
         <v>58</v>
       </c>
@@ -2776,28 +2773,28 @@
       <c r="D10" s="9">
         <v>0</v>
       </c>
-      <c r="E10" s="27">
+      <c r="E10" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F10" s="28">
+      <c r="F10" s="27">
         <v>0.2</v>
       </c>
-      <c r="G10" s="29">
+      <c r="G10" s="28">
         <v>0.8</v>
       </c>
-      <c r="H10" s="26">
+      <c r="H10" s="25">
         <v>5</v>
       </c>
-      <c r="I10" s="26">
+      <c r="I10" s="25">
         <f t="shared" si="1"/>
         <v>1.1</v>
       </c>
-      <c r="J10" s="26">
+      <c r="J10" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K10" s="26">
+      <c r="K10" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2808,33 +2805,33 @@
       <c r="N10" s="17">
         <v>10</v>
       </c>
-      <c r="O10" s="34">
+      <c r="O10" s="33">
         <f t="shared" si="4"/>
         <v>36.57</v>
       </c>
-      <c r="Q10" s="35">
+      <c r="Q10" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R10" s="35">
+      <c r="R10" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T10" s="7">
         <v>32</v>
       </c>
-      <c r="U10" s="37"/>
-      <c r="V10" s="38">
+      <c r="U10" s="36"/>
+      <c r="V10" s="37">
         <f t="shared" si="8"/>
         <v>96</v>
       </c>
-      <c r="W10" s="37"/>
-      <c r="X10" s="37"/>
-      <c r="Y10" s="38">
+      <c r="W10" s="36"/>
+      <c r="X10" s="36"/>
+      <c r="Y10" s="37">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="Z10" s="37"/>
+      <c r="Z10" s="36"/>
       <c r="AD10" s="7" t="s">
         <v>62</v>
       </c>
@@ -2864,28 +2861,28 @@
       <c r="D11" s="9">
         <v>0</v>
       </c>
-      <c r="E11" s="27">
+      <c r="E11" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F11" s="27">
         <v>3.7</v>
       </c>
-      <c r="G11" s="29">
+      <c r="G11" s="28">
         <v>4.2</v>
       </c>
-      <c r="H11" s="26">
+      <c r="H11" s="25">
         <v>5.5</v>
       </c>
-      <c r="I11" s="26">
+      <c r="I11" s="25">
         <f t="shared" si="1"/>
         <v>5.775</v>
       </c>
-      <c r="J11" s="26">
+      <c r="J11" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K11" s="26">
+      <c r="K11" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2896,33 +2893,33 @@
       <c r="N11" s="17">
         <v>13.38</v>
       </c>
-      <c r="O11" s="34">
+      <c r="O11" s="33">
         <f t="shared" si="4"/>
         <v>49.49</v>
       </c>
-      <c r="Q11" s="35">
+      <c r="Q11" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R11" s="35">
+      <c r="R11" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T11" s="7">
         <v>24</v>
       </c>
-      <c r="U11" s="37"/>
-      <c r="V11" s="38">
+      <c r="U11" s="36"/>
+      <c r="V11" s="37">
         <f t="shared" si="8"/>
         <v>360</v>
       </c>
-      <c r="W11" s="37"/>
-      <c r="X11" s="37"/>
-      <c r="Y11" s="38">
+      <c r="W11" s="36"/>
+      <c r="X11" s="36"/>
+      <c r="Y11" s="37">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="Z11" s="37"/>
+      <c r="Z11" s="36"/>
       <c r="AD11" s="7" t="s">
         <v>66</v>
       </c>
@@ -2952,29 +2949,29 @@
       <c r="D12" s="9">
         <v>0</v>
       </c>
-      <c r="E12" s="27">
+      <c r="E12" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F12" s="28">
+      <c r="F12" s="27">
         <v>0.1</v>
       </c>
-      <c r="G12" s="29">
+      <c r="G12" s="28">
         <v>0.2</v>
       </c>
-      <c r="H12" s="26">
+      <c r="H12" s="25">
         <f t="shared" si="7"/>
         <v>0.1375</v>
       </c>
-      <c r="I12" s="26">
+      <c r="I12" s="25">
         <f t="shared" si="1"/>
         <v>0.275</v>
       </c>
-      <c r="J12" s="26">
+      <c r="J12" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K12" s="26">
+      <c r="K12" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2985,33 +2982,33 @@
       <c r="N12" s="17">
         <v>13.38</v>
       </c>
-      <c r="O12" s="34">
+      <c r="O12" s="33">
         <f t="shared" si="4"/>
         <v>53.18</v>
       </c>
-      <c r="Q12" s="35">
+      <c r="Q12" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R12" s="35">
+      <c r="R12" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T12" s="7">
         <v>12</v>
       </c>
-      <c r="U12" s="37"/>
-      <c r="V12" s="38">
+      <c r="U12" s="36"/>
+      <c r="V12" s="37">
         <f t="shared" si="8"/>
         <v>24</v>
       </c>
-      <c r="W12" s="37"/>
-      <c r="X12" s="37"/>
-      <c r="Y12" s="38">
+      <c r="W12" s="36"/>
+      <c r="X12" s="36"/>
+      <c r="Y12" s="37">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="Z12" s="37"/>
+      <c r="Z12" s="36"/>
       <c r="AD12" s="7" t="s">
         <v>70</v>
       </c>
@@ -3041,29 +3038,29 @@
       <c r="D13" s="9">
         <v>0</v>
       </c>
-      <c r="E13" s="27">
+      <c r="E13" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F13" s="28">
+      <c r="F13" s="27">
         <v>0.8</v>
       </c>
-      <c r="G13" s="29">
+      <c r="G13" s="28">
         <v>1.1</v>
       </c>
-      <c r="H13" s="26">
+      <c r="H13" s="25">
         <f t="shared" si="7"/>
         <v>1.1</v>
       </c>
-      <c r="I13" s="26">
+      <c r="I13" s="25">
         <f t="shared" si="1"/>
         <v>1.5125</v>
       </c>
-      <c r="J13" s="26">
+      <c r="J13" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K13" s="26">
+      <c r="K13" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3074,33 +3071,33 @@
       <c r="N13" s="17">
         <v>10.47</v>
       </c>
-      <c r="O13" s="34">
+      <c r="O13" s="33">
         <f t="shared" si="4"/>
         <v>44.18</v>
       </c>
-      <c r="Q13" s="35">
+      <c r="Q13" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R13" s="35">
+      <c r="R13" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T13" s="7">
         <v>15</v>
       </c>
-      <c r="U13" s="37"/>
-      <c r="V13" s="38">
+      <c r="U13" s="36"/>
+      <c r="V13" s="37">
         <f t="shared" si="8"/>
         <v>105</v>
       </c>
-      <c r="W13" s="37"/>
-      <c r="X13" s="37"/>
-      <c r="Y13" s="38">
+      <c r="W13" s="36"/>
+      <c r="X13" s="36"/>
+      <c r="Y13" s="37">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="Z13" s="37"/>
+      <c r="Z13" s="36"/>
       <c r="AD13" s="7" t="s">
         <v>74</v>
       </c>
@@ -3130,29 +3127,29 @@
       <c r="D14" s="9">
         <v>0</v>
       </c>
-      <c r="E14" s="27">
+      <c r="E14" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F14" s="28">
+      <c r="F14" s="27">
         <v>2.5</v>
       </c>
-      <c r="G14" s="29">
+      <c r="G14" s="28">
         <v>2</v>
       </c>
-      <c r="H14" s="26">
+      <c r="H14" s="25">
         <f t="shared" si="7"/>
         <v>3.4375</v>
       </c>
-      <c r="I14" s="26">
+      <c r="I14" s="25">
         <f t="shared" si="1"/>
         <v>3.4375</v>
       </c>
-      <c r="J14" s="26">
+      <c r="J14" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K14" s="26">
+      <c r="K14" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3163,33 +3160,33 @@
       <c r="N14" s="17">
         <v>13.38</v>
       </c>
-      <c r="O14" s="34">
+      <c r="O14" s="33">
         <f t="shared" si="4"/>
         <v>53.18</v>
       </c>
-      <c r="Q14" s="35">
+      <c r="Q14" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R14" s="35">
+      <c r="R14" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T14" s="7">
         <v>12</v>
       </c>
-      <c r="U14" s="37"/>
-      <c r="V14" s="38">
+      <c r="U14" s="36"/>
+      <c r="V14" s="37">
         <f t="shared" si="8"/>
         <v>216</v>
       </c>
-      <c r="W14" s="37"/>
-      <c r="X14" s="37"/>
-      <c r="Y14" s="38">
+      <c r="W14" s="36"/>
+      <c r="X14" s="36"/>
+      <c r="Y14" s="37">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="Z14" s="37"/>
+      <c r="Z14" s="36"/>
       <c r="AD14" s="7" t="s">
         <v>78</v>
       </c>
@@ -3219,7 +3216,7 @@
       <c r="D15" s="9">
         <v>0</v>
       </c>
-      <c r="E15" s="27">
+      <c r="E15" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3229,18 +3226,18 @@
       <c r="G15" s="7">
         <v>0.1</v>
       </c>
-      <c r="H15" s="26">
+      <c r="H15" s="25">
         <v>3</v>
       </c>
-      <c r="I15" s="26">
+      <c r="I15" s="25">
         <f t="shared" si="1"/>
         <v>0.55</v>
       </c>
-      <c r="J15" s="26">
+      <c r="J15" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K15" s="26">
+      <c r="K15" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3251,33 +3248,33 @@
       <c r="N15" s="17">
         <v>10</v>
       </c>
-      <c r="O15" s="34">
+      <c r="O15" s="33">
         <f t="shared" si="4"/>
         <v>34.37</v>
       </c>
-      <c r="Q15" s="35">
+      <c r="Q15" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R15" s="35">
+      <c r="R15" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T15" s="7">
         <v>16</v>
       </c>
-      <c r="U15" s="37"/>
-      <c r="V15" s="38">
+      <c r="U15" s="36"/>
+      <c r="V15" s="37">
         <f t="shared" si="8"/>
         <v>48</v>
       </c>
-      <c r="W15" s="37"/>
-      <c r="X15" s="37"/>
-      <c r="Y15" s="38">
+      <c r="W15" s="36"/>
+      <c r="X15" s="36"/>
+      <c r="Y15" s="37">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="Z15" s="37"/>
+      <c r="Z15" s="36"/>
       <c r="AD15" s="7" t="s">
         <v>82</v>
       </c>
@@ -3307,28 +3304,28 @@
       <c r="D16" s="9">
         <v>0</v>
       </c>
-      <c r="E16" s="27">
+      <c r="E16" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F16" s="28">
+      <c r="F16" s="27">
         <v>1.4</v>
       </c>
-      <c r="G16" s="29">
+      <c r="G16" s="28">
         <v>1.4</v>
       </c>
-      <c r="H16" s="26">
+      <c r="H16" s="25">
         <v>1.9</v>
       </c>
-      <c r="I16" s="26">
+      <c r="I16" s="25">
         <f t="shared" si="1"/>
         <v>1.925</v>
       </c>
-      <c r="J16" s="26">
+      <c r="J16" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K16" s="26">
+      <c r="K16" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3339,33 +3336,33 @@
       <c r="N16" s="17">
         <v>10</v>
       </c>
-      <c r="O16" s="34">
+      <c r="O16" s="33">
         <f t="shared" si="4"/>
         <v>34.37</v>
       </c>
-      <c r="Q16" s="35">
+      <c r="Q16" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R16" s="35">
+      <c r="R16" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T16" s="7">
         <v>16</v>
       </c>
-      <c r="U16" s="38">
+      <c r="U16" s="37">
         <f t="shared" ref="U16:U29" si="10">CEILING(MAX(0,90-MAX(K16,60))*I16/T16,1)*T16</f>
         <v>64</v>
       </c>
-      <c r="V16" s="37"/>
-      <c r="W16" s="37"/>
-      <c r="X16" s="38">
+      <c r="V16" s="36"/>
+      <c r="W16" s="36"/>
+      <c r="X16" s="37">
         <f t="shared" ref="X16:X29" si="11">MIN(CEILING(MAX(0,70-MAX(J16,30))*I16/T16,1)*T16,D16)</f>
         <v>0</v>
       </c>
-      <c r="Y16" s="37"/>
-      <c r="Z16" s="37"/>
+      <c r="Y16" s="36"/>
+      <c r="Z16" s="36"/>
       <c r="AD16" s="7" t="s">
         <v>86</v>
       </c>
@@ -3395,28 +3392,28 @@
       <c r="D17" s="9">
         <v>0</v>
       </c>
-      <c r="E17" s="27">
+      <c r="E17" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F17" s="28">
+      <c r="F17" s="27">
         <v>1</v>
       </c>
-      <c r="G17" s="29">
+      <c r="G17" s="28">
         <v>0.4</v>
       </c>
-      <c r="H17" s="26">
+      <c r="H17" s="25">
         <v>6</v>
       </c>
-      <c r="I17" s="26">
+      <c r="I17" s="25">
         <f t="shared" si="1"/>
         <v>1.375</v>
       </c>
-      <c r="J17" s="26">
+      <c r="J17" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K17" s="26">
+      <c r="K17" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3427,33 +3424,33 @@
       <c r="N17" s="17">
         <v>6</v>
       </c>
-      <c r="O17" s="34">
+      <c r="O17" s="33">
         <f t="shared" si="4"/>
         <v>25.43</v>
       </c>
-      <c r="Q17" s="35">
+      <c r="Q17" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R17" s="35">
+      <c r="R17" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T17" s="7">
         <v>20</v>
       </c>
-      <c r="U17" s="38">
+      <c r="U17" s="37">
         <f t="shared" si="10"/>
         <v>60</v>
       </c>
-      <c r="V17" s="37"/>
-      <c r="W17" s="37"/>
-      <c r="X17" s="38">
+      <c r="V17" s="36"/>
+      <c r="W17" s="36"/>
+      <c r="X17" s="37">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="Y17" s="37"/>
-      <c r="Z17" s="37"/>
+      <c r="Y17" s="36"/>
+      <c r="Z17" s="36"/>
       <c r="AD17" s="7" t="s">
         <v>90</v>
       </c>
@@ -3483,29 +3480,29 @@
       <c r="D18" s="9">
         <v>0</v>
       </c>
-      <c r="E18" s="27">
+      <c r="E18" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F18" s="28">
+      <c r="F18" s="27">
         <v>1</v>
       </c>
-      <c r="G18" s="29">
+      <c r="G18" s="28">
         <v>0.3</v>
       </c>
-      <c r="H18" s="26">
+      <c r="H18" s="25">
         <f t="shared" ref="H18:H21" si="12">MAX(E18,F18)*1.375</f>
         <v>1.375</v>
       </c>
-      <c r="I18" s="26">
+      <c r="I18" s="25">
         <f t="shared" si="1"/>
         <v>1.375</v>
       </c>
-      <c r="J18" s="26">
+      <c r="J18" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K18" s="26">
+      <c r="K18" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3516,33 +3513,33 @@
       <c r="N18" s="17">
         <v>13.38</v>
       </c>
-      <c r="O18" s="34">
+      <c r="O18" s="33">
         <f t="shared" si="4"/>
         <v>49.49</v>
       </c>
-      <c r="Q18" s="35">
+      <c r="Q18" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R18" s="35">
+      <c r="R18" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T18" s="7">
         <v>12</v>
       </c>
-      <c r="U18" s="38">
+      <c r="U18" s="37">
         <f t="shared" si="10"/>
         <v>48</v>
       </c>
-      <c r="V18" s="37"/>
-      <c r="W18" s="37"/>
-      <c r="X18" s="38">
+      <c r="V18" s="36"/>
+      <c r="W18" s="36"/>
+      <c r="X18" s="37">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="Y18" s="37"/>
-      <c r="Z18" s="37"/>
+      <c r="Y18" s="36"/>
+      <c r="Z18" s="36"/>
       <c r="AD18" s="7" t="s">
         <v>94</v>
       </c>
@@ -3572,28 +3569,28 @@
       <c r="D19" s="9">
         <v>0</v>
       </c>
-      <c r="E19" s="27">
+      <c r="E19" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F19" s="28">
+      <c r="F19" s="27">
         <v>0.5</v>
       </c>
-      <c r="G19" s="29">
+      <c r="G19" s="28">
         <v>0.9</v>
       </c>
-      <c r="H19" s="26">
+      <c r="H19" s="25">
         <v>1.4</v>
       </c>
-      <c r="I19" s="26">
+      <c r="I19" s="25">
         <f t="shared" ref="I19:I41" si="13">MAX(F19,G19)*1.375</f>
         <v>1.2375</v>
       </c>
-      <c r="J19" s="26">
+      <c r="J19" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K19" s="26">
+      <c r="K19" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3604,33 +3601,33 @@
       <c r="N19" s="17">
         <v>10</v>
       </c>
-      <c r="O19" s="34">
+      <c r="O19" s="33">
         <f t="shared" si="4"/>
         <v>34.37</v>
       </c>
-      <c r="Q19" s="35">
+      <c r="Q19" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R19" s="35">
+      <c r="R19" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T19" s="7">
         <v>16</v>
       </c>
-      <c r="U19" s="38">
+      <c r="U19" s="37">
         <f t="shared" si="10"/>
         <v>48</v>
       </c>
-      <c r="V19" s="37"/>
-      <c r="W19" s="37"/>
-      <c r="X19" s="38">
+      <c r="V19" s="36"/>
+      <c r="W19" s="36"/>
+      <c r="X19" s="37">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="Y19" s="37"/>
-      <c r="Z19" s="37"/>
+      <c r="Y19" s="36"/>
+      <c r="Z19" s="36"/>
       <c r="AD19" s="7" t="s">
         <v>98</v>
       </c>
@@ -3660,29 +3657,29 @@
       <c r="D20" s="9">
         <v>0</v>
       </c>
-      <c r="E20" s="27">
+      <c r="E20" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F20" s="28">
-        <v>0</v>
-      </c>
-      <c r="G20" s="29">
+      <c r="F20" s="27">
+        <v>0</v>
+      </c>
+      <c r="G20" s="28">
         <v>0.4</v>
       </c>
-      <c r="H20" s="26">
+      <c r="H20" s="25">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="I20" s="26">
+      <c r="I20" s="25">
         <f t="shared" si="13"/>
         <v>0.55</v>
       </c>
-      <c r="J20" s="26">
+      <c r="J20" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K20" s="26">
+      <c r="K20" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3693,33 +3690,33 @@
       <c r="N20" s="17">
         <v>13.38</v>
       </c>
-      <c r="O20" s="34">
+      <c r="O20" s="33">
         <f t="shared" si="4"/>
         <v>49.49</v>
       </c>
-      <c r="Q20" s="35">
+      <c r="Q20" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R20" s="35">
+      <c r="R20" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T20" s="7">
         <v>12</v>
       </c>
-      <c r="U20" s="38">
+      <c r="U20" s="37">
         <f t="shared" si="10"/>
         <v>24</v>
       </c>
-      <c r="V20" s="37"/>
-      <c r="W20" s="37"/>
-      <c r="X20" s="38">
+      <c r="V20" s="36"/>
+      <c r="W20" s="36"/>
+      <c r="X20" s="37">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="Y20" s="37"/>
-      <c r="Z20" s="37"/>
+      <c r="Y20" s="36"/>
+      <c r="Z20" s="36"/>
       <c r="AD20" s="7" t="s">
         <v>102</v>
       </c>
@@ -3749,29 +3746,29 @@
       <c r="D21" s="9">
         <v>0</v>
       </c>
-      <c r="E21" s="27">
+      <c r="E21" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F21" s="28">
+      <c r="F21" s="27">
         <v>1.7</v>
       </c>
-      <c r="G21" s="29">
+      <c r="G21" s="28">
         <v>1.8</v>
       </c>
-      <c r="H21" s="26">
+      <c r="H21" s="25">
         <f t="shared" si="12"/>
         <v>2.3375</v>
       </c>
-      <c r="I21" s="26">
+      <c r="I21" s="25">
         <f t="shared" si="13"/>
         <v>2.475</v>
       </c>
-      <c r="J21" s="26">
+      <c r="J21" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K21" s="26">
+      <c r="K21" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3782,33 +3779,33 @@
       <c r="N21" s="17">
         <v>6.98</v>
       </c>
-      <c r="O21" s="34">
+      <c r="O21" s="33">
         <f t="shared" si="4"/>
         <v>29.72</v>
       </c>
-      <c r="Q21" s="35">
+      <c r="Q21" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R21" s="35">
+      <c r="R21" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T21" s="7">
         <v>21</v>
       </c>
-      <c r="U21" s="38">
+      <c r="U21" s="37">
         <f t="shared" si="10"/>
         <v>84</v>
       </c>
-      <c r="V21" s="37"/>
-      <c r="W21" s="37"/>
-      <c r="X21" s="38">
+      <c r="V21" s="36"/>
+      <c r="W21" s="36"/>
+      <c r="X21" s="37">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="Y21" s="37"/>
-      <c r="Z21" s="37"/>
+      <c r="Y21" s="36"/>
+      <c r="Z21" s="36"/>
       <c r="AD21" s="7" t="s">
         <v>106</v>
       </c>
@@ -3838,28 +3835,28 @@
       <c r="D22" s="9">
         <v>0</v>
       </c>
-      <c r="E22" s="27">
+      <c r="E22" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F22" s="28">
+      <c r="F22" s="27">
         <v>0.5</v>
       </c>
-      <c r="G22" s="29">
+      <c r="G22" s="28">
         <v>0.5</v>
       </c>
-      <c r="H22" s="26">
+      <c r="H22" s="25">
         <v>2</v>
       </c>
-      <c r="I22" s="26">
+      <c r="I22" s="25">
         <f t="shared" si="13"/>
         <v>0.6875</v>
       </c>
-      <c r="J22" s="26">
+      <c r="J22" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K22" s="26">
+      <c r="K22" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3870,33 +3867,33 @@
       <c r="N22" s="17">
         <v>9</v>
       </c>
-      <c r="O22" s="34">
+      <c r="O22" s="33">
         <f t="shared" si="4"/>
         <v>37.52</v>
       </c>
-      <c r="Q22" s="35">
+      <c r="Q22" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R22" s="35">
+      <c r="R22" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T22" s="7">
         <v>14</v>
       </c>
-      <c r="U22" s="38">
+      <c r="U22" s="37">
         <f t="shared" si="10"/>
         <v>28</v>
       </c>
-      <c r="V22" s="37"/>
-      <c r="W22" s="37"/>
-      <c r="X22" s="38">
+      <c r="V22" s="36"/>
+      <c r="W22" s="36"/>
+      <c r="X22" s="37">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="Y22" s="37"/>
-      <c r="Z22" s="37"/>
+      <c r="Y22" s="36"/>
+      <c r="Z22" s="36"/>
       <c r="AD22" s="7" t="s">
         <v>110</v>
       </c>
@@ -3926,29 +3923,29 @@
       <c r="D23" s="9">
         <v>0</v>
       </c>
-      <c r="E23" s="27">
+      <c r="E23" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F23" s="28">
+      <c r="F23" s="27">
         <v>0.5</v>
       </c>
-      <c r="G23" s="29">
+      <c r="G23" s="28">
         <v>0.7</v>
       </c>
-      <c r="H23" s="26">
+      <c r="H23" s="25">
         <f>MAX(E23,F23)*1.375</f>
         <v>0.6875</v>
       </c>
-      <c r="I23" s="26">
+      <c r="I23" s="25">
         <f t="shared" si="13"/>
         <v>0.9625</v>
       </c>
-      <c r="J23" s="26">
+      <c r="J23" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K23" s="26">
+      <c r="K23" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3959,33 +3956,33 @@
       <c r="N23" s="17">
         <v>10</v>
       </c>
-      <c r="O23" s="34">
+      <c r="O23" s="33">
         <f t="shared" si="4"/>
         <v>34.37</v>
       </c>
-      <c r="Q23" s="35">
+      <c r="Q23" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R23" s="35">
+      <c r="R23" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T23" s="7">
         <v>16</v>
       </c>
-      <c r="U23" s="38">
+      <c r="U23" s="37">
         <f t="shared" si="10"/>
         <v>32</v>
       </c>
-      <c r="V23" s="37"/>
-      <c r="W23" s="37"/>
-      <c r="X23" s="38">
+      <c r="V23" s="36"/>
+      <c r="W23" s="36"/>
+      <c r="X23" s="37">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="Y23" s="37"/>
-      <c r="Z23" s="37"/>
+      <c r="Y23" s="36"/>
+      <c r="Z23" s="36"/>
       <c r="AD23" s="7" t="s">
         <v>114</v>
       </c>
@@ -4015,29 +4012,29 @@
       <c r="D24" s="9">
         <v>0</v>
       </c>
-      <c r="E24" s="27">
+      <c r="E24" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F24" s="29">
+      <c r="F24" s="28">
         <v>0.7</v>
       </c>
-      <c r="G24" s="29">
+      <c r="G24" s="28">
         <v>1</v>
       </c>
-      <c r="H24" s="26">
+      <c r="H24" s="25">
         <f>MAX(E24,F24)*1.375</f>
         <v>0.9625</v>
       </c>
-      <c r="I24" s="26">
+      <c r="I24" s="25">
         <f t="shared" si="13"/>
         <v>1.375</v>
       </c>
-      <c r="J24" s="26">
+      <c r="J24" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K24" s="26">
+      <c r="K24" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4048,33 +4045,33 @@
       <c r="N24" s="17">
         <v>10</v>
       </c>
-      <c r="O24" s="34">
+      <c r="O24" s="33">
         <f t="shared" si="4"/>
         <v>34.37</v>
       </c>
-      <c r="Q24" s="35">
+      <c r="Q24" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R24" s="35">
+      <c r="R24" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T24" s="7">
         <v>16</v>
       </c>
-      <c r="U24" s="38">
+      <c r="U24" s="37">
         <f t="shared" si="10"/>
         <v>48</v>
       </c>
-      <c r="V24" s="37"/>
-      <c r="W24" s="37"/>
-      <c r="X24" s="38">
+      <c r="V24" s="36"/>
+      <c r="W24" s="36"/>
+      <c r="X24" s="37">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="Y24" s="37"/>
-      <c r="Z24" s="37"/>
+      <c r="Y24" s="36"/>
+      <c r="Z24" s="36"/>
       <c r="AD24" s="7" t="s">
         <v>118</v>
       </c>
@@ -4104,28 +4101,28 @@
       <c r="D25" s="9">
         <v>0</v>
       </c>
-      <c r="E25" s="27">
+      <c r="E25" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F25" s="29">
+      <c r="F25" s="28">
         <v>1.2</v>
       </c>
-      <c r="G25" s="29">
+      <c r="G25" s="28">
         <v>1.4</v>
       </c>
-      <c r="H25" s="26">
+      <c r="H25" s="25">
         <v>2.5</v>
       </c>
-      <c r="I25" s="26">
+      <c r="I25" s="25">
         <f t="shared" si="13"/>
         <v>1.925</v>
       </c>
-      <c r="J25" s="26">
+      <c r="J25" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K25" s="26">
+      <c r="K25" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4136,33 +4133,33 @@
       <c r="N25" s="17">
         <v>6</v>
       </c>
-      <c r="O25" s="34">
+      <c r="O25" s="33">
         <f t="shared" si="4"/>
         <v>25.43</v>
       </c>
-      <c r="Q25" s="35">
+      <c r="Q25" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R25" s="35">
+      <c r="R25" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T25" s="7">
         <v>20</v>
       </c>
-      <c r="U25" s="38">
+      <c r="U25" s="37">
         <f t="shared" si="10"/>
         <v>60</v>
       </c>
-      <c r="V25" s="37"/>
-      <c r="W25" s="37"/>
-      <c r="X25" s="38">
+      <c r="V25" s="36"/>
+      <c r="W25" s="36"/>
+      <c r="X25" s="37">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="Y25" s="37"/>
-      <c r="Z25" s="37"/>
+      <c r="Y25" s="36"/>
+      <c r="Z25" s="36"/>
       <c r="AD25" s="7" t="s">
         <v>122</v>
       </c>
@@ -4192,28 +4189,28 @@
       <c r="D26" s="9">
         <v>0</v>
       </c>
-      <c r="E26" s="27">
+      <c r="E26" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F26" s="29">
+      <c r="F26" s="28">
         <v>0.7</v>
       </c>
-      <c r="G26" s="29">
+      <c r="G26" s="28">
         <v>0.7</v>
       </c>
-      <c r="H26" s="26">
+      <c r="H26" s="25">
         <v>4</v>
       </c>
-      <c r="I26" s="26">
+      <c r="I26" s="25">
         <f t="shared" si="13"/>
         <v>0.9625</v>
       </c>
-      <c r="J26" s="26">
+      <c r="J26" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K26" s="26">
+      <c r="K26" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4224,33 +4221,33 @@
       <c r="N26" s="17">
         <v>6.98</v>
       </c>
-      <c r="O26" s="34">
+      <c r="O26" s="33">
         <f t="shared" si="4"/>
         <v>29.72</v>
       </c>
-      <c r="Q26" s="35">
+      <c r="Q26" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R26" s="35">
+      <c r="R26" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T26" s="7">
         <v>21</v>
       </c>
-      <c r="U26" s="38">
+      <c r="U26" s="37">
         <f t="shared" si="10"/>
         <v>42</v>
       </c>
-      <c r="V26" s="37"/>
-      <c r="W26" s="37"/>
-      <c r="X26" s="38">
+      <c r="V26" s="36"/>
+      <c r="W26" s="36"/>
+      <c r="X26" s="37">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="Y26" s="37"/>
-      <c r="Z26" s="37"/>
+      <c r="Y26" s="36"/>
+      <c r="Z26" s="36"/>
       <c r="AD26" s="7" t="s">
         <v>126</v>
       </c>
@@ -4280,29 +4277,29 @@
       <c r="D27" s="9">
         <v>0</v>
       </c>
-      <c r="E27" s="27">
+      <c r="E27" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F27" s="29">
+      <c r="F27" s="28">
         <v>1.5</v>
       </c>
-      <c r="G27" s="29">
+      <c r="G27" s="28">
         <v>1.2</v>
       </c>
-      <c r="H27" s="26">
+      <c r="H27" s="25">
         <f>MAX(E27,F27)*1.375</f>
         <v>2.0625</v>
       </c>
-      <c r="I27" s="26">
+      <c r="I27" s="25">
         <f t="shared" si="13"/>
         <v>2.0625</v>
       </c>
-      <c r="J27" s="26">
+      <c r="J27" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K27" s="26">
+      <c r="K27" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4313,33 +4310,33 @@
       <c r="N27" s="17">
         <v>10</v>
       </c>
-      <c r="O27" s="34">
+      <c r="O27" s="33">
         <f t="shared" si="4"/>
         <v>34.37</v>
       </c>
-      <c r="Q27" s="35">
+      <c r="Q27" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R27" s="35">
+      <c r="R27" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T27" s="7">
         <v>16</v>
       </c>
-      <c r="U27" s="38">
+      <c r="U27" s="37">
         <f t="shared" si="10"/>
         <v>64</v>
       </c>
-      <c r="V27" s="37"/>
-      <c r="W27" s="37"/>
-      <c r="X27" s="38">
+      <c r="V27" s="36"/>
+      <c r="W27" s="36"/>
+      <c r="X27" s="37">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="Y27" s="37"/>
-      <c r="Z27" s="37"/>
+      <c r="Y27" s="36"/>
+      <c r="Z27" s="36"/>
       <c r="AD27" s="7" t="s">
         <v>130</v>
       </c>
@@ -4369,29 +4366,29 @@
       <c r="D28" s="9">
         <v>0</v>
       </c>
-      <c r="E28" s="27">
+      <c r="E28" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F28" s="28">
+      <c r="F28" s="27">
         <v>1.1</v>
       </c>
-      <c r="G28" s="29">
+      <c r="G28" s="28">
         <v>0.5</v>
       </c>
-      <c r="H28" s="26">
+      <c r="H28" s="25">
         <f>MAX(E28,F28)*1.375</f>
         <v>1.5125</v>
       </c>
-      <c r="I28" s="26">
+      <c r="I28" s="25">
         <f t="shared" si="13"/>
         <v>1.5125</v>
       </c>
-      <c r="J28" s="26">
+      <c r="J28" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K28" s="26">
+      <c r="K28" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4402,33 +4399,33 @@
       <c r="N28" s="17">
         <v>13.38</v>
       </c>
-      <c r="O28" s="34">
+      <c r="O28" s="33">
         <f t="shared" si="4"/>
         <v>49.49</v>
       </c>
-      <c r="Q28" s="35">
+      <c r="Q28" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R28" s="35">
+      <c r="R28" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T28" s="7">
         <v>12</v>
       </c>
-      <c r="U28" s="38">
+      <c r="U28" s="37">
         <f t="shared" si="10"/>
         <v>48</v>
       </c>
-      <c r="V28" s="37"/>
-      <c r="W28" s="37"/>
-      <c r="X28" s="38">
+      <c r="V28" s="36"/>
+      <c r="W28" s="36"/>
+      <c r="X28" s="37">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="Y28" s="37"/>
-      <c r="Z28" s="37"/>
+      <c r="Y28" s="36"/>
+      <c r="Z28" s="36"/>
       <c r="AD28" s="7" t="s">
         <v>134</v>
       </c>
@@ -4458,29 +4455,29 @@
       <c r="D29" s="9">
         <v>0</v>
       </c>
-      <c r="E29" s="27">
+      <c r="E29" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F29" s="28">
+      <c r="F29" s="27">
         <v>0.8</v>
       </c>
-      <c r="G29" s="29">
+      <c r="G29" s="28">
         <v>1</v>
       </c>
-      <c r="H29" s="26">
+      <c r="H29" s="25">
         <f>MAX(E29,F29)*1.375</f>
         <v>1.1</v>
       </c>
-      <c r="I29" s="26">
+      <c r="I29" s="25">
         <f t="shared" si="13"/>
         <v>1.375</v>
       </c>
-      <c r="J29" s="26">
+      <c r="J29" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K29" s="26">
+      <c r="K29" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4491,33 +4488,33 @@
       <c r="N29" s="17">
         <v>10</v>
       </c>
-      <c r="O29" s="34">
+      <c r="O29" s="33">
         <f t="shared" si="4"/>
         <v>34.37</v>
       </c>
-      <c r="Q29" s="35">
+      <c r="Q29" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R29" s="35">
+      <c r="R29" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T29" s="7">
         <v>16</v>
       </c>
-      <c r="U29" s="38">
+      <c r="U29" s="37">
         <f t="shared" si="10"/>
         <v>48</v>
       </c>
-      <c r="V29" s="37"/>
-      <c r="W29" s="37"/>
-      <c r="X29" s="38">
+      <c r="V29" s="36"/>
+      <c r="W29" s="36"/>
+      <c r="X29" s="37">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="Y29" s="37"/>
-      <c r="Z29" s="37"/>
+      <c r="Y29" s="36"/>
+      <c r="Z29" s="36"/>
       <c r="AD29" s="7" t="s">
         <v>138</v>
       </c>
@@ -4547,29 +4544,29 @@
       <c r="D30" s="9">
         <v>0</v>
       </c>
-      <c r="E30" s="30">
+      <c r="E30" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F30" s="31">
+      <c r="F30" s="30">
         <v>0.1</v>
       </c>
-      <c r="G30" s="32">
-        <v>0</v>
-      </c>
-      <c r="H30" s="26">
+      <c r="G30" s="31">
+        <v>0</v>
+      </c>
+      <c r="H30" s="25">
         <f>MAX(E30,F30)*1.375</f>
         <v>0.1375</v>
       </c>
-      <c r="I30" s="26">
+      <c r="I30" s="25">
         <f t="shared" si="13"/>
         <v>0.1375</v>
       </c>
-      <c r="J30" s="26">
+      <c r="J30" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K30" s="26">
+      <c r="K30" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4580,33 +4577,33 @@
       <c r="N30" s="17">
         <v>10</v>
       </c>
-      <c r="O30" s="34">
+      <c r="O30" s="33">
         <f t="shared" si="4"/>
         <v>36.57</v>
       </c>
-      <c r="Q30" s="35">
+      <c r="Q30" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R30" s="35">
+      <c r="R30" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T30" s="7">
         <v>16</v>
       </c>
-      <c r="U30" s="38">
+      <c r="U30" s="37">
         <f t="shared" ref="U30:U44" si="14">CEILING(MAX(0,90-MAX(K30,60))*I30/T30,1)*T30</f>
         <v>16</v>
       </c>
-      <c r="V30" s="37"/>
-      <c r="W30" s="37"/>
-      <c r="X30" s="38">
+      <c r="V30" s="36"/>
+      <c r="W30" s="36"/>
+      <c r="X30" s="37">
         <f t="shared" ref="X30:X44" si="15">MIN(CEILING(MAX(0,70-MAX(J30,30))*I30/T30,1)*T30,D30)</f>
         <v>0</v>
       </c>
-      <c r="Y30" s="37"/>
-      <c r="Z30" s="37"/>
+      <c r="Y30" s="36"/>
+      <c r="Z30" s="36"/>
       <c r="AD30" s="7" t="s">
         <v>142</v>
       </c>
@@ -4636,29 +4633,29 @@
       <c r="D31" s="9">
         <v>0</v>
       </c>
-      <c r="E31" s="30">
+      <c r="E31" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F31" s="28">
+      <c r="F31" s="27">
         <v>0.1</v>
       </c>
-      <c r="G31" s="29">
+      <c r="G31" s="28">
         <v>0.1</v>
       </c>
-      <c r="H31" s="26">
+      <c r="H31" s="25">
         <f>MAX(E31,F31)*1.375</f>
         <v>0.1375</v>
       </c>
-      <c r="I31" s="26">
+      <c r="I31" s="25">
         <f t="shared" si="13"/>
         <v>0.1375</v>
       </c>
-      <c r="J31" s="26">
+      <c r="J31" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K31" s="26">
+      <c r="K31" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4669,33 +4666,33 @@
       <c r="N31" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="O31" s="34">
+      <c r="O31" s="33">
         <f t="shared" si="4"/>
         <v>30</v>
       </c>
-      <c r="Q31" s="35">
+      <c r="Q31" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R31" s="35">
+      <c r="R31" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T31" s="7">
         <v>30</v>
       </c>
-      <c r="U31" s="38">
+      <c r="U31" s="37">
         <f t="shared" si="14"/>
         <v>30</v>
       </c>
-      <c r="V31" s="37"/>
-      <c r="W31" s="37"/>
-      <c r="X31" s="38">
+      <c r="V31" s="36"/>
+      <c r="W31" s="36"/>
+      <c r="X31" s="37">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="Y31" s="37"/>
-      <c r="Z31" s="37"/>
+      <c r="Y31" s="36"/>
+      <c r="Z31" s="36"/>
       <c r="AD31" s="7" t="s">
         <v>148</v>
       </c>
@@ -4725,7 +4722,7 @@
       <c r="D32" s="9">
         <v>0</v>
       </c>
-      <c r="E32" s="30">
+      <c r="E32" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4735,18 +4732,18 @@
       <c r="G32" s="7">
         <v>2.5</v>
       </c>
-      <c r="H32" s="26">
+      <c r="H32" s="25">
         <v>3.5</v>
       </c>
-      <c r="I32" s="26">
+      <c r="I32" s="25">
         <f t="shared" si="13"/>
         <v>3.85</v>
       </c>
-      <c r="J32" s="26">
+      <c r="J32" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K32" s="26">
+      <c r="K32" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4757,33 +4754,33 @@
       <c r="N32" s="17">
         <v>10</v>
       </c>
-      <c r="O32" s="34">
+      <c r="O32" s="33">
         <f t="shared" si="4"/>
         <v>34.37</v>
       </c>
-      <c r="Q32" s="35">
+      <c r="Q32" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R32" s="35">
+      <c r="R32" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T32" s="7">
         <v>16</v>
       </c>
-      <c r="U32" s="38">
+      <c r="U32" s="37">
         <f t="shared" si="14"/>
         <v>128</v>
       </c>
-      <c r="V32" s="37"/>
-      <c r="W32" s="37"/>
-      <c r="X32" s="38">
+      <c r="V32" s="36"/>
+      <c r="W32" s="36"/>
+      <c r="X32" s="37">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="Y32" s="37"/>
-      <c r="Z32" s="37"/>
+      <c r="Y32" s="36"/>
+      <c r="Z32" s="36"/>
       <c r="AD32" s="7" t="s">
         <v>152</v>
       </c>
@@ -4813,7 +4810,7 @@
       <c r="D33" s="9">
         <v>0</v>
       </c>
-      <c r="E33" s="30">
+      <c r="E33" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4823,18 +4820,18 @@
       <c r="G33" s="7">
         <v>0.4</v>
       </c>
-      <c r="H33" s="26">
+      <c r="H33" s="25">
         <v>2</v>
       </c>
-      <c r="I33" s="26">
+      <c r="I33" s="25">
         <f t="shared" si="13"/>
         <v>1.1</v>
       </c>
-      <c r="J33" s="26">
+      <c r="J33" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K33" s="26">
+      <c r="K33" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4845,33 +4842,33 @@
       <c r="N33" s="17">
         <v>10</v>
       </c>
-      <c r="O33" s="34">
+      <c r="O33" s="33">
         <f t="shared" si="4"/>
         <v>34.37</v>
       </c>
-      <c r="Q33" s="35">
+      <c r="Q33" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R33" s="35">
+      <c r="R33" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T33" s="7">
         <v>16</v>
       </c>
-      <c r="U33" s="38">
+      <c r="U33" s="37">
         <f t="shared" si="14"/>
         <v>48</v>
       </c>
-      <c r="V33" s="37"/>
-      <c r="W33" s="37"/>
-      <c r="X33" s="38">
+      <c r="V33" s="36"/>
+      <c r="W33" s="36"/>
+      <c r="X33" s="37">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="Y33" s="37"/>
-      <c r="Z33" s="37"/>
+      <c r="Y33" s="36"/>
+      <c r="Z33" s="36"/>
       <c r="AD33" s="8" t="s">
         <v>156</v>
       </c>
@@ -4901,7 +4898,7 @@
       <c r="D34" s="9">
         <v>0</v>
       </c>
-      <c r="E34" s="30">
+      <c r="E34" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4911,18 +4908,18 @@
       <c r="G34" s="7">
         <v>1.1</v>
       </c>
-      <c r="H34" s="26">
+      <c r="H34" s="25">
         <v>3</v>
       </c>
-      <c r="I34" s="26">
+      <c r="I34" s="25">
         <f t="shared" si="13"/>
         <v>1.5125</v>
       </c>
-      <c r="J34" s="26">
+      <c r="J34" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K34" s="26">
+      <c r="K34" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4933,33 +4930,33 @@
       <c r="N34" s="17">
         <v>10</v>
       </c>
-      <c r="O34" s="34">
+      <c r="O34" s="33">
         <f t="shared" si="4"/>
         <v>36.57</v>
       </c>
-      <c r="Q34" s="35">
+      <c r="Q34" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R34" s="35">
+      <c r="R34" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T34" s="7">
         <v>32</v>
       </c>
-      <c r="U34" s="38">
+      <c r="U34" s="37">
         <f t="shared" si="14"/>
         <v>64</v>
       </c>
-      <c r="V34" s="37"/>
-      <c r="W34" s="37"/>
-      <c r="X34" s="38">
+      <c r="V34" s="36"/>
+      <c r="W34" s="36"/>
+      <c r="X34" s="37">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="Y34" s="37"/>
-      <c r="Z34" s="37"/>
+      <c r="Y34" s="36"/>
+      <c r="Z34" s="36"/>
       <c r="AD34" s="7" t="s">
         <v>160</v>
       </c>
@@ -4989,7 +4986,7 @@
       <c r="D35" s="9">
         <v>0</v>
       </c>
-      <c r="E35" s="30">
+      <c r="E35" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4999,18 +4996,18 @@
       <c r="G35" s="7">
         <v>2.2</v>
       </c>
-      <c r="H35" s="26">
+      <c r="H35" s="25">
         <v>4.5</v>
       </c>
-      <c r="I35" s="26">
+      <c r="I35" s="25">
         <f t="shared" si="13"/>
         <v>3.025</v>
       </c>
-      <c r="J35" s="26">
+      <c r="J35" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K35" s="26">
+      <c r="K35" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -5021,33 +5018,33 @@
       <c r="N35" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="O35" s="34">
+      <c r="O35" s="33">
         <f t="shared" si="4"/>
         <v>19</v>
       </c>
-      <c r="Q35" s="35">
+      <c r="Q35" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R35" s="35">
+      <c r="R35" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T35" s="7">
         <v>32</v>
       </c>
-      <c r="U35" s="38">
+      <c r="U35" s="37">
         <f t="shared" si="14"/>
         <v>96</v>
       </c>
-      <c r="V35" s="37"/>
-      <c r="W35" s="37"/>
-      <c r="X35" s="38">
+      <c r="V35" s="36"/>
+      <c r="W35" s="36"/>
+      <c r="X35" s="37">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="Y35" s="37"/>
-      <c r="Z35" s="37"/>
+      <c r="Y35" s="36"/>
+      <c r="Z35" s="36"/>
       <c r="AD35" s="7" t="s">
         <v>166</v>
       </c>
@@ -5077,7 +5074,7 @@
       <c r="D36" s="9">
         <v>0</v>
       </c>
-      <c r="E36" s="30">
+      <c r="E36" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5087,18 +5084,18 @@
       <c r="G36" s="7">
         <v>0.6</v>
       </c>
-      <c r="H36" s="26">
+      <c r="H36" s="25">
         <v>1</v>
       </c>
-      <c r="I36" s="26">
+      <c r="I36" s="25">
         <f t="shared" si="13"/>
         <v>0.9625</v>
       </c>
-      <c r="J36" s="26">
+      <c r="J36" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K36" s="26">
+      <c r="K36" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -5109,33 +5106,33 @@
       <c r="N36" s="17">
         <v>10</v>
       </c>
-      <c r="O36" s="34">
+      <c r="O36" s="33">
         <f t="shared" si="4"/>
         <v>34.37</v>
       </c>
-      <c r="Q36" s="35">
+      <c r="Q36" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R36" s="35">
+      <c r="R36" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T36" s="7">
         <v>16</v>
       </c>
-      <c r="U36" s="38">
+      <c r="U36" s="37">
         <f t="shared" si="14"/>
         <v>32</v>
       </c>
-      <c r="V36" s="37"/>
-      <c r="W36" s="37"/>
-      <c r="X36" s="38">
+      <c r="V36" s="36"/>
+      <c r="W36" s="36"/>
+      <c r="X36" s="37">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="Y36" s="37"/>
-      <c r="Z36" s="37"/>
+      <c r="Y36" s="36"/>
+      <c r="Z36" s="36"/>
       <c r="AD36" s="7" t="s">
         <v>170</v>
       </c>
@@ -5165,7 +5162,7 @@
       <c r="D37" s="9">
         <v>0</v>
       </c>
-      <c r="E37" s="30">
+      <c r="E37" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5175,18 +5172,18 @@
       <c r="G37" s="7">
         <v>0.5</v>
       </c>
-      <c r="H37" s="26">
+      <c r="H37" s="25">
         <v>1</v>
       </c>
-      <c r="I37" s="26">
+      <c r="I37" s="25">
         <f t="shared" si="13"/>
         <v>0.6875</v>
       </c>
-      <c r="J37" s="26">
+      <c r="J37" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K37" s="26">
+      <c r="K37" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -5197,33 +5194,33 @@
       <c r="N37" s="17">
         <v>10</v>
       </c>
-      <c r="O37" s="34">
+      <c r="O37" s="33">
         <f t="shared" si="4"/>
         <v>34.37</v>
       </c>
-      <c r="Q37" s="35">
+      <c r="Q37" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R37" s="35">
+      <c r="R37" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T37" s="7">
         <v>16</v>
       </c>
-      <c r="U37" s="38">
+      <c r="U37" s="37">
         <f t="shared" si="14"/>
         <v>32</v>
       </c>
-      <c r="V37" s="37"/>
-      <c r="W37" s="37"/>
-      <c r="X37" s="38">
+      <c r="V37" s="36"/>
+      <c r="W37" s="36"/>
+      <c r="X37" s="37">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="Y37" s="37"/>
-      <c r="Z37" s="37"/>
+      <c r="Y37" s="36"/>
+      <c r="Z37" s="36"/>
       <c r="AD37" s="8" t="s">
         <v>174</v>
       </c>
@@ -5253,7 +5250,7 @@
       <c r="D38" s="9">
         <v>0</v>
       </c>
-      <c r="E38" s="27">
+      <c r="E38" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5263,18 +5260,18 @@
       <c r="G38" s="7">
         <v>1</v>
       </c>
-      <c r="H38" s="26">
+      <c r="H38" s="25">
         <v>3.5</v>
       </c>
-      <c r="I38" s="26">
+      <c r="I38" s="25">
         <f t="shared" si="13"/>
         <v>3.4375</v>
       </c>
-      <c r="J38" s="26">
+      <c r="J38" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K38" s="26">
+      <c r="K38" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -5285,33 +5282,33 @@
       <c r="N38" s="17">
         <v>10</v>
       </c>
-      <c r="O38" s="34">
+      <c r="O38" s="33">
         <f t="shared" si="4"/>
         <v>34.37</v>
       </c>
-      <c r="Q38" s="35">
+      <c r="Q38" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R38" s="35">
+      <c r="R38" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T38" s="7">
         <v>16</v>
       </c>
-      <c r="U38" s="38">
+      <c r="U38" s="37">
         <f t="shared" si="14"/>
         <v>112</v>
       </c>
-      <c r="V38" s="37"/>
-      <c r="W38" s="37"/>
-      <c r="X38" s="38">
+      <c r="V38" s="36"/>
+      <c r="W38" s="36"/>
+      <c r="X38" s="37">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="Y38" s="37"/>
-      <c r="Z38" s="37"/>
+      <c r="Y38" s="36"/>
+      <c r="Z38" s="36"/>
       <c r="AD38" s="7" t="s">
         <v>178</v>
       </c>
@@ -5341,7 +5338,7 @@
       <c r="D39" s="9">
         <v>0</v>
       </c>
-      <c r="E39" s="27">
+      <c r="E39" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5351,19 +5348,19 @@
       <c r="G39" s="7">
         <v>0.3</v>
       </c>
-      <c r="H39" s="26">
+      <c r="H39" s="25">
         <f t="shared" ref="H39:H51" si="16">MAX(E39,F39)*1.375</f>
         <v>0.55</v>
       </c>
-      <c r="I39" s="26">
+      <c r="I39" s="25">
         <f t="shared" si="13"/>
         <v>0.55</v>
       </c>
-      <c r="J39" s="26">
+      <c r="J39" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K39" s="26">
+      <c r="K39" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -5374,33 +5371,33 @@
       <c r="N39" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="O39" s="34">
+      <c r="O39" s="33">
         <f t="shared" si="4"/>
         <v>30.8</v>
       </c>
-      <c r="Q39" s="35">
+      <c r="Q39" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R39" s="35">
+      <c r="R39" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T39" s="7">
         <v>20</v>
       </c>
-      <c r="U39" s="38">
+      <c r="U39" s="37">
         <f t="shared" si="14"/>
         <v>20</v>
       </c>
-      <c r="V39" s="37"/>
-      <c r="W39" s="37"/>
-      <c r="X39" s="38">
+      <c r="V39" s="36"/>
+      <c r="W39" s="36"/>
+      <c r="X39" s="37">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="Y39" s="37"/>
-      <c r="Z39" s="37"/>
+      <c r="Y39" s="36"/>
+      <c r="Z39" s="36"/>
       <c r="AD39" s="7" t="s">
         <v>184</v>
       </c>
@@ -5430,7 +5427,7 @@
       <c r="D40" s="9">
         <v>0</v>
       </c>
-      <c r="E40" s="27">
+      <c r="E40" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5440,19 +5437,19 @@
       <c r="G40" s="7">
         <v>0.1</v>
       </c>
-      <c r="H40" s="26">
+      <c r="H40" s="25">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="I40" s="26">
+      <c r="I40" s="25">
         <f t="shared" si="13"/>
         <v>0.1375</v>
       </c>
-      <c r="J40" s="26">
+      <c r="J40" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K40" s="26">
+      <c r="K40" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -5463,33 +5460,33 @@
       <c r="N40" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="O40" s="34">
+      <c r="O40" s="33">
         <f t="shared" si="4"/>
         <v>32.8</v>
       </c>
-      <c r="Q40" s="35">
+      <c r="Q40" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R40" s="35">
+      <c r="R40" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T40" s="7">
         <v>20</v>
       </c>
-      <c r="U40" s="38">
+      <c r="U40" s="37">
         <f t="shared" si="14"/>
         <v>20</v>
       </c>
-      <c r="V40" s="37"/>
-      <c r="W40" s="37"/>
-      <c r="X40" s="38">
+      <c r="V40" s="36"/>
+      <c r="W40" s="36"/>
+      <c r="X40" s="37">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="Y40" s="37"/>
-      <c r="Z40" s="37"/>
+      <c r="Y40" s="36"/>
+      <c r="Z40" s="36"/>
       <c r="AD40" s="7" t="s">
         <v>188</v>
       </c>
@@ -5519,7 +5516,7 @@
       <c r="D41" s="9">
         <v>0</v>
       </c>
-      <c r="E41" s="27">
+      <c r="E41" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5529,18 +5526,18 @@
       <c r="G41" s="7">
         <v>0</v>
       </c>
-      <c r="H41" s="26">
+      <c r="H41" s="25">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="I41" s="26">
+      <c r="I41" s="25">
         <v>1</v>
       </c>
-      <c r="J41" s="26">
+      <c r="J41" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K41" s="26">
+      <c r="K41" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -5550,33 +5547,33 @@
       <c r="N41" s="17">
         <v>10</v>
       </c>
-      <c r="O41" s="34">
+      <c r="O41" s="33">
         <f t="shared" si="4"/>
         <v>36.57</v>
       </c>
-      <c r="Q41" s="35">
+      <c r="Q41" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R41" s="35">
+      <c r="R41" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T41" s="7">
         <v>16</v>
       </c>
-      <c r="U41" s="38">
+      <c r="U41" s="37">
         <f t="shared" si="14"/>
         <v>32</v>
       </c>
-      <c r="V41" s="37"/>
-      <c r="W41" s="37"/>
-      <c r="X41" s="38">
+      <c r="V41" s="36"/>
+      <c r="W41" s="36"/>
+      <c r="X41" s="37">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="Y41" s="37"/>
-      <c r="Z41" s="37"/>
+      <c r="Y41" s="36"/>
+      <c r="Z41" s="36"/>
       <c r="AD41" s="7" t="s">
         <v>192</v>
       </c>
@@ -5606,7 +5603,7 @@
       <c r="D42" s="9">
         <v>0</v>
       </c>
-      <c r="E42" s="27">
+      <c r="E42" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5616,18 +5613,18 @@
       <c r="G42" s="7">
         <v>0</v>
       </c>
-      <c r="H42" s="26">
+      <c r="H42" s="25">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="I42" s="26">
+      <c r="I42" s="25">
         <v>1</v>
       </c>
-      <c r="J42" s="26">
+      <c r="J42" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K42" s="26">
+      <c r="K42" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -5637,33 +5634,33 @@
       <c r="N42" s="17">
         <v>10</v>
       </c>
-      <c r="O42" s="34">
+      <c r="O42" s="33">
         <f t="shared" si="4"/>
         <v>36.57</v>
       </c>
-      <c r="Q42" s="35">
+      <c r="Q42" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R42" s="35">
+      <c r="R42" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T42" s="7">
         <v>16</v>
       </c>
-      <c r="U42" s="38">
+      <c r="U42" s="37">
         <f t="shared" si="14"/>
         <v>32</v>
       </c>
-      <c r="V42" s="37"/>
-      <c r="W42" s="37"/>
-      <c r="X42" s="38">
+      <c r="V42" s="36"/>
+      <c r="W42" s="36"/>
+      <c r="X42" s="37">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="Y42" s="37"/>
-      <c r="Z42" s="37"/>
+      <c r="Y42" s="36"/>
+      <c r="Z42" s="36"/>
       <c r="AD42" s="7" t="s">
         <v>196</v>
       </c>
@@ -5693,7 +5690,7 @@
       <c r="D43" s="9">
         <v>0</v>
       </c>
-      <c r="E43" s="27">
+      <c r="E43" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5703,18 +5700,18 @@
       <c r="G43" s="7">
         <v>0</v>
       </c>
-      <c r="H43" s="26">
+      <c r="H43" s="25">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="I43" s="26">
+      <c r="I43" s="25">
         <v>1</v>
       </c>
-      <c r="J43" s="26">
+      <c r="J43" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K43" s="26">
+      <c r="K43" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -5724,33 +5721,33 @@
       <c r="N43" s="7">
         <v>5</v>
       </c>
-      <c r="O43" s="34">
+      <c r="O43" s="33">
         <f t="shared" si="4"/>
         <v>18.3</v>
       </c>
-      <c r="Q43" s="35">
+      <c r="Q43" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R43" s="35">
+      <c r="R43" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T43" s="7">
         <v>32</v>
       </c>
-      <c r="U43" s="38">
+      <c r="U43" s="37">
         <f t="shared" si="14"/>
         <v>32</v>
       </c>
-      <c r="V43" s="37"/>
-      <c r="W43" s="37"/>
-      <c r="X43" s="38">
+      <c r="V43" s="36"/>
+      <c r="W43" s="36"/>
+      <c r="X43" s="37">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="Y43" s="37"/>
-      <c r="Z43" s="37"/>
+      <c r="Y43" s="36"/>
+      <c r="Z43" s="36"/>
       <c r="AD43" s="7" t="s">
         <v>200</v>
       </c>
@@ -5780,7 +5777,7 @@
       <c r="D44" s="9">
         <v>0</v>
       </c>
-      <c r="E44" s="27">
+      <c r="E44" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5790,18 +5787,18 @@
       <c r="G44" s="7">
         <v>0</v>
       </c>
-      <c r="H44" s="26">
+      <c r="H44" s="25">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="I44" s="26">
+      <c r="I44" s="25">
         <v>1</v>
       </c>
-      <c r="J44" s="26">
+      <c r="J44" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K44" s="26">
+      <c r="K44" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -5811,33 +5808,33 @@
       <c r="N44" s="7">
         <v>3</v>
       </c>
-      <c r="O44" s="34">
+      <c r="O44" s="33">
         <f t="shared" si="4"/>
         <v>13</v>
       </c>
-      <c r="Q44" s="35">
+      <c r="Q44" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R44" s="35">
+      <c r="R44" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T44" s="7">
         <v>72</v>
       </c>
-      <c r="U44" s="38">
+      <c r="U44" s="37">
         <f t="shared" si="14"/>
         <v>72</v>
       </c>
-      <c r="V44" s="37"/>
-      <c r="W44" s="37"/>
-      <c r="X44" s="38">
+      <c r="V44" s="36"/>
+      <c r="W44" s="36"/>
+      <c r="X44" s="37">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="Y44" s="37"/>
-      <c r="Z44" s="37"/>
+      <c r="Y44" s="36"/>
+      <c r="Z44" s="36"/>
       <c r="AD44" s="7" t="s">
         <v>204</v>
       </c>
@@ -5855,10 +5852,10 @@
       </c>
     </row>
     <row r="45" ht="25" customHeight="1" spans="1:34">
-      <c r="A45" s="24" t="s">
+      <c r="A45" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="B45" s="24" t="s">
+      <c r="B45" s="7" t="s">
         <v>207</v>
       </c>
       <c r="C45" s="9">
@@ -5867,7 +5864,7 @@
       <c r="D45" s="9">
         <v>0</v>
       </c>
-      <c r="E45" s="27">
+      <c r="E45" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5877,62 +5874,62 @@
       <c r="G45" s="7">
         <v>0</v>
       </c>
-      <c r="H45" s="26">
+      <c r="H45" s="25">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="I45" s="26">
+      <c r="I45" s="25">
         <v>1</v>
       </c>
-      <c r="J45" s="26">
+      <c r="J45" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K45" s="26">
+      <c r="K45" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M45" s="24">
+      <c r="M45" s="7">
         <v>39</v>
       </c>
-      <c r="N45" s="24">
+      <c r="N45" s="7">
         <v>12</v>
       </c>
-      <c r="O45" s="34">
-        <f>M45+N45</f>
+      <c r="O45" s="33">
+        <f t="shared" si="4"/>
         <v>51</v>
       </c>
-      <c r="Q45" s="35">
+      <c r="Q45" s="34">
         <f t="shared" ref="Q45:Q51" si="17">M45*C45</f>
         <v>0</v>
       </c>
-      <c r="R45" s="35">
+      <c r="R45" s="34">
         <f t="shared" ref="R45:R51" si="18">M45*D45</f>
         <v>0</v>
       </c>
-      <c r="T45" s="24">
+      <c r="T45" s="7">
         <v>18</v>
       </c>
-      <c r="U45" s="38">
+      <c r="U45" s="37">
         <f t="shared" ref="U45:U51" si="19">CEILING(MAX(0,90-MAX(K45,60))*I45/T45,1)*T45</f>
         <v>36</v>
       </c>
-      <c r="V45" s="37"/>
-      <c r="W45" s="37"/>
-      <c r="X45" s="38">
+      <c r="V45" s="36"/>
+      <c r="W45" s="36"/>
+      <c r="X45" s="37">
         <f t="shared" ref="X45:X51" si="20">MIN(CEILING(MAX(0,70-MAX(J45,30))*I45/T45,1)*T45,D45)</f>
         <v>0</v>
       </c>
-      <c r="Y45" s="37"/>
-      <c r="Z45" s="37"/>
-      <c r="AD45" s="24" t="s">
+      <c r="Y45" s="36"/>
+      <c r="Z45" s="36"/>
+      <c r="AD45" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="AE45" s="24" t="s">
+      <c r="AE45" s="7" t="s">
         <v>209</v>
       </c>
       <c r="AF45" s="7">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="AG45" s="7">
         <v>37</v>
@@ -5942,10 +5939,10 @@
       </c>
     </row>
     <row r="46" ht="25" customHeight="1" spans="1:34">
-      <c r="A46" s="24" t="s">
+      <c r="A46" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="B46" s="24" t="s">
+      <c r="B46" s="7" t="s">
         <v>211</v>
       </c>
       <c r="C46" s="9">
@@ -5954,7 +5951,7 @@
       <c r="D46" s="9">
         <v>0</v>
       </c>
-      <c r="E46" s="27">
+      <c r="E46" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5964,62 +5961,62 @@
       <c r="G46" s="7">
         <v>0</v>
       </c>
-      <c r="H46" s="26">
+      <c r="H46" s="25">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="I46" s="26">
+      <c r="I46" s="25">
         <v>1</v>
       </c>
-      <c r="J46" s="26">
+      <c r="J46" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K46" s="26">
+      <c r="K46" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M46" s="24">
+      <c r="M46" s="7">
         <v>19.5</v>
       </c>
       <c r="N46" s="17">
         <v>6</v>
       </c>
-      <c r="O46" s="34">
+      <c r="O46" s="33">
         <f t="shared" ref="O46:O51" si="21">M46+N46</f>
         <v>25.5</v>
       </c>
-      <c r="Q46" s="35">
+      <c r="Q46" s="34">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="R46" s="35">
+      <c r="R46" s="34">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="T46" s="7">
-        <v>36</v>
-      </c>
-      <c r="U46" s="38">
+        <v>20</v>
+      </c>
+      <c r="U46" s="37">
         <f t="shared" si="19"/>
-        <v>36</v>
-      </c>
-      <c r="V46" s="37"/>
-      <c r="W46" s="37"/>
-      <c r="X46" s="38">
+        <v>40</v>
+      </c>
+      <c r="V46" s="36"/>
+      <c r="W46" s="36"/>
+      <c r="X46" s="37">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="Y46" s="37"/>
-      <c r="Z46" s="37"/>
-      <c r="AD46" s="24" t="s">
+      <c r="Y46" s="36"/>
+      <c r="Z46" s="36"/>
+      <c r="AD46" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="AE46" s="24" t="s">
+      <c r="AE46" s="7" t="s">
         <v>213</v>
       </c>
       <c r="AF46" s="7">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="AG46" s="7">
         <v>37</v>
@@ -6029,10 +6026,10 @@
       </c>
     </row>
     <row r="47" ht="25" customHeight="1" spans="1:34">
-      <c r="A47" s="24" t="s">
+      <c r="A47" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="B47" s="24" t="s">
+      <c r="B47" s="7" t="s">
         <v>215</v>
       </c>
       <c r="C47" s="9">
@@ -6041,7 +6038,7 @@
       <c r="D47" s="9">
         <v>0</v>
       </c>
-      <c r="E47" s="27">
+      <c r="E47" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6051,62 +6048,62 @@
       <c r="G47" s="7">
         <v>0</v>
       </c>
-      <c r="H47" s="26">
+      <c r="H47" s="25">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="I47" s="26">
+      <c r="I47" s="25">
         <v>1</v>
       </c>
-      <c r="J47" s="26">
+      <c r="J47" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K47" s="26">
+      <c r="K47" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M47" s="24">
+      <c r="M47" s="7">
         <v>19.5</v>
       </c>
       <c r="N47" s="17">
         <v>6</v>
       </c>
-      <c r="O47" s="34">
+      <c r="O47" s="33">
         <f t="shared" si="21"/>
         <v>25.5</v>
       </c>
-      <c r="Q47" s="35">
+      <c r="Q47" s="34">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="R47" s="35">
+      <c r="R47" s="34">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="T47" s="7">
-        <v>36</v>
-      </c>
-      <c r="U47" s="38">
+        <v>20</v>
+      </c>
+      <c r="U47" s="37">
         <f t="shared" si="19"/>
-        <v>36</v>
-      </c>
-      <c r="V47" s="37"/>
-      <c r="W47" s="37"/>
-      <c r="X47" s="38">
+        <v>40</v>
+      </c>
+      <c r="V47" s="36"/>
+      <c r="W47" s="36"/>
+      <c r="X47" s="37">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="Y47" s="37"/>
-      <c r="Z47" s="37"/>
-      <c r="AD47" s="24" t="s">
+      <c r="Y47" s="36"/>
+      <c r="Z47" s="36"/>
+      <c r="AD47" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="AE47" s="24" t="s">
+      <c r="AE47" s="7" t="s">
         <v>217</v>
       </c>
       <c r="AF47" s="7">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="AG47" s="7">
         <v>37</v>
@@ -6116,10 +6113,10 @@
       </c>
     </row>
     <row r="48" ht="25" customHeight="1" spans="1:34">
-      <c r="A48" s="24" t="s">
+      <c r="A48" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="B48" s="24" t="s">
+      <c r="B48" s="7" t="s">
         <v>219</v>
       </c>
       <c r="C48" s="9">
@@ -6128,7 +6125,7 @@
       <c r="D48" s="9">
         <v>0</v>
       </c>
-      <c r="E48" s="27">
+      <c r="E48" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6138,58 +6135,58 @@
       <c r="G48" s="7">
         <v>0</v>
       </c>
-      <c r="H48" s="26">
+      <c r="H48" s="25">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="I48" s="26">
+      <c r="I48" s="25">
         <v>1</v>
       </c>
-      <c r="J48" s="26">
+      <c r="J48" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K48" s="26">
+      <c r="K48" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M48" s="24">
+      <c r="M48" s="7">
         <v>19.5</v>
       </c>
       <c r="N48" s="17">
         <v>6</v>
       </c>
-      <c r="O48" s="34">
+      <c r="O48" s="33">
         <f t="shared" si="21"/>
         <v>25.5</v>
       </c>
-      <c r="Q48" s="35">
+      <c r="Q48" s="34">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="R48" s="35">
+      <c r="R48" s="34">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="T48" s="7">
-        <v>36</v>
-      </c>
-      <c r="U48" s="38">
+        <v>20</v>
+      </c>
+      <c r="U48" s="37">
         <f t="shared" si="19"/>
-        <v>36</v>
-      </c>
-      <c r="V48" s="37"/>
-      <c r="W48" s="37"/>
-      <c r="X48" s="38">
+        <v>40</v>
+      </c>
+      <c r="V48" s="36"/>
+      <c r="W48" s="36"/>
+      <c r="X48" s="37">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="Y48" s="37"/>
-      <c r="Z48" s="37"/>
-      <c r="AD48" s="24" t="s">
+      <c r="Y48" s="36"/>
+      <c r="Z48" s="36"/>
+      <c r="AD48" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="AE48" s="24" t="s">
+      <c r="AE48" s="7" t="s">
         <v>221</v>
       </c>
       <c r="AF48" s="7">
@@ -6203,10 +6200,10 @@
       </c>
     </row>
     <row r="49" ht="25" customHeight="1" spans="1:34">
-      <c r="A49" s="24" t="s">
+      <c r="A49" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="B49" s="24" t="s">
+      <c r="B49" s="7" t="s">
         <v>223</v>
       </c>
       <c r="C49" s="9">
@@ -6215,7 +6212,7 @@
       <c r="D49" s="9">
         <v>0</v>
       </c>
-      <c r="E49" s="27">
+      <c r="E49" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6225,18 +6222,18 @@
       <c r="G49" s="7">
         <v>0</v>
       </c>
-      <c r="H49" s="26">
+      <c r="H49" s="25">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="I49" s="26">
+      <c r="I49" s="25">
         <v>1</v>
       </c>
-      <c r="J49" s="26">
+      <c r="J49" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K49" s="26">
+      <c r="K49" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -6246,37 +6243,37 @@
       <c r="N49" s="17">
         <v>10</v>
       </c>
-      <c r="O49" s="34">
+      <c r="O49" s="33">
         <f t="shared" si="21"/>
         <v>34.37</v>
       </c>
-      <c r="Q49" s="35">
+      <c r="Q49" s="34">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="R49" s="35">
+      <c r="R49" s="34">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="T49" s="7">
         <v>16</v>
       </c>
-      <c r="U49" s="38">
+      <c r="U49" s="37">
         <f t="shared" si="19"/>
         <v>32</v>
       </c>
-      <c r="V49" s="37"/>
-      <c r="W49" s="37"/>
-      <c r="X49" s="38">
+      <c r="V49" s="36"/>
+      <c r="W49" s="36"/>
+      <c r="X49" s="37">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="Y49" s="37"/>
-      <c r="Z49" s="37"/>
-      <c r="AD49" s="24" t="s">
+      <c r="Y49" s="36"/>
+      <c r="Z49" s="36"/>
+      <c r="AD49" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="AE49" s="24" t="s">
+      <c r="AE49" s="7" t="s">
         <v>225</v>
       </c>
       <c r="AF49" s="7">
@@ -6290,10 +6287,10 @@
       </c>
     </row>
     <row r="50" ht="25" customHeight="1" spans="1:34">
-      <c r="A50" s="24" t="s">
+      <c r="A50" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="B50" s="24" t="s">
+      <c r="B50" s="7" t="s">
         <v>227</v>
       </c>
       <c r="C50" s="9">
@@ -6302,7 +6299,7 @@
       <c r="D50" s="9">
         <v>0</v>
       </c>
-      <c r="E50" s="27">
+      <c r="E50" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6312,18 +6309,18 @@
       <c r="G50" s="7">
         <v>0</v>
       </c>
-      <c r="H50" s="26">
+      <c r="H50" s="25">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="I50" s="26">
+      <c r="I50" s="25">
         <v>1</v>
       </c>
-      <c r="J50" s="26">
+      <c r="J50" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K50" s="26">
+      <c r="K50" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -6333,37 +6330,37 @@
       <c r="N50" s="17">
         <v>10</v>
       </c>
-      <c r="O50" s="34">
+      <c r="O50" s="33">
         <f t="shared" si="21"/>
         <v>34.37</v>
       </c>
-      <c r="Q50" s="35">
+      <c r="Q50" s="34">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="R50" s="35">
+      <c r="R50" s="34">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="T50" s="7">
         <v>16</v>
       </c>
-      <c r="U50" s="38">
+      <c r="U50" s="37">
         <f t="shared" si="19"/>
         <v>32</v>
       </c>
-      <c r="V50" s="37"/>
-      <c r="W50" s="37"/>
-      <c r="X50" s="38">
+      <c r="V50" s="36"/>
+      <c r="W50" s="36"/>
+      <c r="X50" s="37">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="Y50" s="37"/>
-      <c r="Z50" s="37"/>
-      <c r="AD50" s="24" t="s">
+      <c r="Y50" s="36"/>
+      <c r="Z50" s="36"/>
+      <c r="AD50" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="AE50" s="24" t="s">
+      <c r="AE50" s="7" t="s">
         <v>229</v>
       </c>
       <c r="AF50" s="7">
@@ -6377,10 +6374,10 @@
       </c>
     </row>
     <row r="51" ht="25" customHeight="1" spans="1:34">
-      <c r="A51" s="24" t="s">
+      <c r="A51" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="B51" s="24" t="s">
+      <c r="B51" s="7" t="s">
         <v>231</v>
       </c>
       <c r="C51" s="9">
@@ -6389,7 +6386,7 @@
       <c r="D51" s="9">
         <v>0</v>
       </c>
-      <c r="E51" s="27">
+      <c r="E51" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6399,18 +6396,18 @@
       <c r="G51" s="7">
         <v>0</v>
       </c>
-      <c r="H51" s="26">
+      <c r="H51" s="25">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="I51" s="26">
+      <c r="I51" s="25">
         <v>1</v>
       </c>
-      <c r="J51" s="26">
+      <c r="J51" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K51" s="26">
+      <c r="K51" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -6420,37 +6417,37 @@
       <c r="N51" s="7">
         <v>5</v>
       </c>
-      <c r="O51" s="34">
+      <c r="O51" s="33">
         <f t="shared" si="21"/>
         <v>18.3</v>
       </c>
-      <c r="Q51" s="35">
+      <c r="Q51" s="34">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="R51" s="35">
+      <c r="R51" s="34">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="T51" s="24">
+      <c r="T51" s="7">
         <v>32</v>
       </c>
-      <c r="U51" s="38">
+      <c r="U51" s="37">
         <f t="shared" si="19"/>
         <v>32</v>
       </c>
-      <c r="V51" s="37"/>
-      <c r="W51" s="37"/>
-      <c r="X51" s="38">
+      <c r="V51" s="36"/>
+      <c r="W51" s="36"/>
+      <c r="X51" s="37">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="Y51" s="37"/>
-      <c r="Z51" s="37"/>
-      <c r="AD51" s="24" t="s">
+      <c r="Y51" s="36"/>
+      <c r="Z51" s="36"/>
+      <c r="AD51" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="AE51" s="24" t="s">
+      <c r="AE51" s="7" t="s">
         <v>233</v>
       </c>
       <c r="AF51" s="7">
@@ -6484,7 +6481,7 @@
     <row r="70" ht="25" customHeight="1"/>
     <row r="71" ht="25" customHeight="1"/>
   </sheetData>
-  <autoFilter ref="A1:AH44">
+  <autoFilter ref="A1:AH51">
     <extLst/>
   </autoFilter>
   <conditionalFormatting sqref="J45">

</xml_diff>

<commit_message>
Build project and prepare for upload
</commit_message>
<xml_diff>
--- a/dist/产品库存及周转统计.xlsx
+++ b/dist/产品库存及周转统计.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="20900"/>
+    <workbookView windowWidth="28000" windowHeight="15860"/>
   </bookViews>
   <sheets>
     <sheet name="产品库存" sheetId="1" r:id="rId1"/>
@@ -531,7 +531,7 @@
     <t>5</t>
   </si>
   <si>
-    <t>BedSideCaddy-2pockets-Greyipcs-New</t>
+    <t>BedSideCaddy-2pockets-Grey1pcs-New</t>
   </si>
   <si>
     <t>X004RETHGT</t>
@@ -1934,11 +1934,11 @@
   <dimension ref="A1:AH71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="T7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="S22" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AE13" sqref="AE13"/>
+      <selection pane="bottomRight" activeCell="AI34" sqref="AI34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>

</xml_diff>